<commit_message>
VS: additional excel sample data
more interesting sample data
</commit_message>
<xml_diff>
--- a/ExtSACP01-sample-data.xlsx
+++ b/ExtSACP01-sample-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sap-my.sharepoint.com/personal/vlad-andrei_sladariu_sap_com/Documents/====Projects/2023-01 Barilla/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I065468\ds2022\git\btp-global-center-of-excellence-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{B5346E15-9417-4FAE-B733-AEC435231D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C06152C-BB7D-4404-9086-1AF3444A3CAE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD474DBF-8C8B-474B-9A2B-6401BF9F8077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9705" yWindow="2445" windowWidth="18945" windowHeight="9945" xr2:uid="{7E0579ED-CA7F-4DF0-9A6A-38ABD20310C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E0579ED-CA7F-4DF0-9A6A-38ABD20310C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="13">
   <si>
     <t>Account</t>
   </si>
@@ -442,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6281C07A-A037-40BC-A7D1-478E141F5CC8}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A98" sqref="A98:E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,6 +455,14 @@
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -488,7 +496,7 @@
         <v>202301</v>
       </c>
       <c r="E2">
-        <v>-30000</v>
+        <v>-28500</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -499,13 +507,13 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>202301</v>
+        <v>202302</v>
       </c>
       <c r="E3">
-        <v>1000</v>
+        <v>-32100.000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -516,13 +524,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>202301</v>
+        <v>202303</v>
       </c>
       <c r="E4">
-        <v>-30</v>
+        <v>-29100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -533,81 +541,81 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>202301</v>
+        <v>202201</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>-33000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>202301</v>
+        <v>202202</v>
       </c>
       <c r="E6">
-        <v>-30000</v>
+        <v>-31500</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>202301</v>
+        <v>202203</v>
       </c>
       <c r="E7">
-        <v>1000</v>
+        <v>-30900</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>202301</v>
+        <v>202204</v>
       </c>
       <c r="E8">
-        <v>-30</v>
+        <v>-30600</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>202301</v>
+        <v>202205</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>-28200</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -621,10 +629,10 @@
         <v>5</v>
       </c>
       <c r="D10">
-        <v>202302</v>
+        <v>202206</v>
       </c>
       <c r="E10">
-        <v>-30000</v>
+        <v>-31800</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -635,13 +643,13 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>202302</v>
+        <v>202207</v>
       </c>
       <c r="E11">
-        <v>950</v>
+        <v>-27600</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -652,13 +660,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>202302</v>
+        <v>202208</v>
       </c>
       <c r="E12">
-        <v>-30</v>
+        <v>-27000</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -669,81 +677,81 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>202302</v>
+        <v>202209</v>
       </c>
       <c r="E13">
-        <v>105</v>
+        <v>-31500</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14">
-        <v>202302</v>
+        <v>202210</v>
       </c>
       <c r="E14">
-        <v>-30000</v>
+        <v>-30900</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>202302</v>
+        <v>202211</v>
       </c>
       <c r="E15">
-        <v>950</v>
+        <v>-31800</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>202302</v>
+        <v>202212</v>
       </c>
       <c r="E16">
-        <v>-30</v>
+        <v>-30900</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17">
-        <v>202302</v>
+        <v>202301</v>
       </c>
       <c r="E17">
-        <v>105</v>
+        <v>-29.4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -754,13 +762,13 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>202303</v>
+        <v>202302</v>
       </c>
       <c r="E18">
-        <v>-30000</v>
+        <v>-28.799999999999997</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -771,13 +779,13 @@
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>202303</v>
       </c>
       <c r="E19">
-        <v>1050</v>
+        <v>-30.6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -791,10 +799,10 @@
         <v>4</v>
       </c>
       <c r="D20">
-        <v>202303</v>
+        <v>202201</v>
       </c>
       <c r="E20">
-        <v>-30</v>
+        <v>-30.900000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -805,291 +813,1515 @@
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>202303</v>
+        <v>202202</v>
       </c>
       <c r="E21">
-        <v>95</v>
+        <v>-31.200000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>202303</v>
+        <v>202203</v>
       </c>
       <c r="E22">
-        <v>-30000</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>202303</v>
+        <v>202204</v>
       </c>
       <c r="E23">
-        <v>1050</v>
+        <v>-31.200000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24">
-        <v>202303</v>
+        <v>202205</v>
       </c>
       <c r="E24">
-        <v>-30</v>
+        <v>-29.7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25">
-        <v>202303</v>
+        <v>202206</v>
       </c>
       <c r="E25">
-        <v>95</v>
+        <v>-29.7</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26">
-        <v>202304</v>
+        <v>202207</v>
       </c>
       <c r="E26">
-        <v>-30000</v>
+        <v>-30.3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D27">
-        <v>202304</v>
+        <v>202208</v>
       </c>
       <c r="E27">
-        <v>1000</v>
+        <v>-31.200000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28">
-        <v>202304</v>
+        <v>202209</v>
       </c>
       <c r="E28">
-        <v>-30</v>
+        <v>-28.5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29">
-        <v>202304</v>
+        <v>202210</v>
       </c>
       <c r="E29">
-        <v>100</v>
+        <v>-28.5</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30">
-        <v>202305</v>
+        <v>202211</v>
       </c>
       <c r="E30">
-        <v>-30000</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D31">
-        <v>202305</v>
+        <v>202212</v>
       </c>
       <c r="E31">
-        <v>1000</v>
+        <v>-31.200000000000003</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32">
-        <v>202305</v>
+        <v>202301</v>
       </c>
       <c r="E32">
-        <v>-30</v>
+        <v>101.61</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
       </c>
       <c r="D33">
-        <v>202305</v>
+        <v>202302</v>
       </c>
       <c r="E33">
-        <v>100</v>
+        <v>103.46</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D34">
-        <v>202306</v>
+        <v>202303</v>
       </c>
       <c r="E34">
-        <v>-30000</v>
+        <v>106.22</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D35">
-        <v>202306</v>
+        <v>202201</v>
       </c>
       <c r="E35">
-        <v>1000</v>
+        <v>99.62</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>202306</v>
+        <v>202202</v>
       </c>
       <c r="E36">
-        <v>-30</v>
+        <v>101.43</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
         <v>3</v>
       </c>
       <c r="D37">
+        <v>202203</v>
+      </c>
+      <c r="E37">
+        <v>104.14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>202204</v>
+      </c>
+      <c r="E38">
+        <v>103.99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>202205</v>
+      </c>
+      <c r="E39">
+        <v>102.42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>202206</v>
+      </c>
+      <c r="E40">
+        <v>97.24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>202207</v>
+      </c>
+      <c r="E41">
+        <v>97.52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>202208</v>
+      </c>
+      <c r="E42">
+        <v>95.85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>202209</v>
+      </c>
+      <c r="E43">
+        <v>96.99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>202210</v>
+      </c>
+      <c r="E44">
+        <v>97.95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>202211</v>
+      </c>
+      <c r="E45">
+        <v>101.58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>202212</v>
+      </c>
+      <c r="E46">
+        <v>102.56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47">
+        <v>202301</v>
+      </c>
+      <c r="E47">
+        <v>9015</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48">
+        <v>202302</v>
+      </c>
+      <c r="E48">
+        <v>7915.0000000000036</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49">
+        <v>202303</v>
+      </c>
+      <c r="E49">
+        <v>6495</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50">
+        <v>202201</v>
+      </c>
+      <c r="E50">
+        <v>10574.999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51">
+        <v>202202</v>
+      </c>
+      <c r="E51">
+        <v>9574.9999999999964</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52">
+        <v>202203</v>
+      </c>
+      <c r="E52">
+        <v>8265</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53">
+        <v>202204</v>
+      </c>
+      <c r="E53">
+        <v>8285.0000000000036</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54">
+        <v>202205</v>
+      </c>
+      <c r="E54">
+        <v>8425</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55">
+        <v>202206</v>
+      </c>
+      <c r="E55">
+        <v>11620.000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56">
+        <v>202207</v>
+      </c>
+      <c r="E56">
+        <v>10990.000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57">
+        <v>202208</v>
+      </c>
+      <c r="E57">
+        <v>12225.000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58">
+        <v>202209</v>
+      </c>
+      <c r="E58">
+        <v>11205.000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59">
+        <v>202210</v>
+      </c>
+      <c r="E59">
+        <v>11399.999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <v>202211</v>
+      </c>
+      <c r="E60">
+        <v>9150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61">
+        <v>202212</v>
+      </c>
+      <c r="E61">
+        <v>9039.9999999999982</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62">
+        <v>202301</v>
+      </c>
+      <c r="E62">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63">
+        <v>202302</v>
+      </c>
+      <c r="E63">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <v>202303</v>
+      </c>
+      <c r="E64">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65">
+        <v>202304</v>
+      </c>
+      <c r="E65">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>202305</v>
+      </c>
+      <c r="E66">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67">
         <v>202306</v>
       </c>
-      <c r="E37">
-        <v>100</v>
+      <c r="E67">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68">
+        <v>202307</v>
+      </c>
+      <c r="E68">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69">
+        <v>202308</v>
+      </c>
+      <c r="E69">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70">
+        <v>202309</v>
+      </c>
+      <c r="E70">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71">
+        <v>202310</v>
+      </c>
+      <c r="E71">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72">
+        <v>202311</v>
+      </c>
+      <c r="E72">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>202312</v>
+      </c>
+      <c r="E73">
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74">
+        <v>202301</v>
+      </c>
+      <c r="E74">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75">
+        <v>202302</v>
+      </c>
+      <c r="E75">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76">
+        <v>202303</v>
+      </c>
+      <c r="E76">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77">
+        <v>202304</v>
+      </c>
+      <c r="E77">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78">
+        <v>202305</v>
+      </c>
+      <c r="E78">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79">
+        <v>202306</v>
+      </c>
+      <c r="E79">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>7</v>
+      </c>
+      <c r="B80" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80">
+        <v>202307</v>
+      </c>
+      <c r="E80">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81">
+        <v>202308</v>
+      </c>
+      <c r="E81">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>7</v>
+      </c>
+      <c r="B82" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82">
+        <v>202309</v>
+      </c>
+      <c r="E82">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>7</v>
+      </c>
+      <c r="B83" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83">
+        <v>202310</v>
+      </c>
+      <c r="E83">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84">
+        <v>202311</v>
+      </c>
+      <c r="E84">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85">
+        <v>202312</v>
+      </c>
+      <c r="E85">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>7</v>
+      </c>
+      <c r="B86" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" t="s">
+        <v>3</v>
+      </c>
+      <c r="D86">
+        <v>202301</v>
+      </c>
+      <c r="E86">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>7</v>
+      </c>
+      <c r="B87" t="s">
+        <v>10</v>
+      </c>
+      <c r="C87" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87">
+        <v>202302</v>
+      </c>
+      <c r="E87">
+        <v>103.46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88">
+        <v>202303</v>
+      </c>
+      <c r="E88">
+        <v>106.22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89">
+        <v>202304</v>
+      </c>
+      <c r="E89">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>7</v>
+      </c>
+      <c r="B90" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90">
+        <v>202305</v>
+      </c>
+      <c r="E90">
+        <v>104.47</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>7</v>
+      </c>
+      <c r="B91" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" t="s">
+        <v>3</v>
+      </c>
+      <c r="D91">
+        <v>202306</v>
+      </c>
+      <c r="E91">
+        <v>99.18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>7</v>
+      </c>
+      <c r="B92" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92">
+        <v>202307</v>
+      </c>
+      <c r="E92">
+        <v>99.47</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>7</v>
+      </c>
+      <c r="B93" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93" t="s">
+        <v>3</v>
+      </c>
+      <c r="D93">
+        <v>202308</v>
+      </c>
+      <c r="E93">
+        <v>97.77</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>7</v>
+      </c>
+      <c r="B94" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" t="s">
+        <v>3</v>
+      </c>
+      <c r="D94">
+        <v>202309</v>
+      </c>
+      <c r="E94">
+        <v>98.93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>7</v>
+      </c>
+      <c r="B95" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95">
+        <v>202310</v>
+      </c>
+      <c r="E95">
+        <v>99.91</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>7</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96">
+        <v>202311</v>
+      </c>
+      <c r="E96">
+        <v>103.61</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>7</v>
+      </c>
+      <c r="B97" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" t="s">
+        <v>3</v>
+      </c>
+      <c r="D97">
+        <v>202312</v>
+      </c>
+      <c r="E97">
+        <v>104.61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98">
+        <v>202301</v>
+      </c>
+      <c r="E98">
+        <v>10787</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>7</v>
+      </c>
+      <c r="B99" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" t="s">
+        <v>12</v>
+      </c>
+      <c r="D99">
+        <v>202302</v>
+      </c>
+      <c r="E99">
+        <v>9767</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" t="s">
+        <v>12</v>
+      </c>
+      <c r="D100">
+        <v>202303</v>
+      </c>
+      <c r="E100">
+        <v>8430</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101">
+        <v>202304</v>
+      </c>
+      <c r="E101">
+        <v>8451</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>7</v>
+      </c>
+      <c r="B102" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102">
+        <v>202305</v>
+      </c>
+      <c r="E102">
+        <v>8594</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>7</v>
+      </c>
+      <c r="B103" t="s">
+        <v>10</v>
+      </c>
+      <c r="C103" t="s">
+        <v>12</v>
+      </c>
+      <c r="D103">
+        <v>202306</v>
+      </c>
+      <c r="E103">
+        <v>11852</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104">
+        <v>202307</v>
+      </c>
+      <c r="E104">
+        <v>11210</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105" t="s">
+        <v>12</v>
+      </c>
+      <c r="D105">
+        <v>202308</v>
+      </c>
+      <c r="E105">
+        <v>12470</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>7</v>
+      </c>
+      <c r="B106" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106">
+        <v>202309</v>
+      </c>
+      <c r="E106">
+        <v>11429</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>7</v>
+      </c>
+      <c r="B107" t="s">
+        <v>10</v>
+      </c>
+      <c r="C107" t="s">
+        <v>12</v>
+      </c>
+      <c r="D107">
+        <v>202310</v>
+      </c>
+      <c r="E107">
+        <v>11628</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>7</v>
+      </c>
+      <c r="B108" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108" t="s">
+        <v>12</v>
+      </c>
+      <c r="D108">
+        <v>202311</v>
+      </c>
+      <c r="E108">
+        <v>9333</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>7</v>
+      </c>
+      <c r="B109" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109">
+        <v>202312</v>
+      </c>
+      <c r="E109">
+        <v>9221</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{6281C07A-A037-40BC-A7D1-478E141F5CC8}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E37">
-      <sortCondition ref="D1"/>
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>